<commit_message>
Added class OtherMethods and some refactoring
</commit_message>
<xml_diff>
--- a/Result/List.xlsx
+++ b/Result/List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming_study\Selenium\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07ABCAA5-A286-4BAC-8AD7-37F1C7AF0FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4717DB1-30F7-46DE-A4C1-6E1821DCAA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25380" yWindow="2130" windowWidth="21600" windowHeight="11505" xr2:uid="{75B22889-0432-4817-A9E3-86FBEBFAA7E3}"/>
+    <workbookView xWindow="3495" yWindow="1380" windowWidth="21600" windowHeight="11505" xr2:uid="{EDB3CD6A-F251-496A-BCEB-ADEA57E75F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Results List" sheetId="2" r:id="rId1"/>
@@ -35,192 +35,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
-  <si>
-    <t>Усадьба</t>
-  </si>
-  <si>
-    <t>Кафе</t>
-  </si>
-  <si>
-    <t>Молодежная ул., 5-б</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 01:00</t>
-  </si>
-  <si>
-    <t>Открыто</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 01:00</t>
-  </si>
-  <si>
-    <t>Бахус</t>
-  </si>
-  <si>
-    <t>ул. Энтузиастов, 24</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 23:00</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 23:00</t>
-  </si>
-  <si>
-    <t>Ретро Кафе</t>
-  </si>
-  <si>
-    <t>Индустриальная ул., 12</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 06:00 (чт)</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 06:00 (чт)</t>
-  </si>
-  <si>
-    <t>Grand Кафе</t>
-  </si>
-  <si>
-    <t>Ресторан</t>
-  </si>
-  <si>
-    <t>пр. Курчатова, 4а</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 00:00</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 00:00</t>
-  </si>
-  <si>
-    <t>Крепость</t>
-  </si>
-  <si>
-    <t>пр. Мира, 44</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 02:00</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 02:00</t>
-  </si>
-  <si>
-    <t>Старая мельница</t>
-  </si>
-  <si>
-    <t>пер. Пушкина, 1</t>
-  </si>
-  <si>
-    <t>Кафе "Тихий Дон"</t>
-  </si>
-  <si>
-    <t>ул. Степная, 73</t>
-  </si>
-  <si>
-    <t>Старый Рояль</t>
-  </si>
-  <si>
-    <t>ул. Ленина, 5</t>
-  </si>
-  <si>
-    <t>Шашлычный Мир</t>
-  </si>
-  <si>
-    <t>ул. Энтузиастов, 43б</t>
-  </si>
-  <si>
-    <t>Скоро закроется: 19:40 ⋅ Откроется в 10:00 (чт)</t>
-  </si>
-  <si>
-    <t>Скоро закроется:</t>
-  </si>
-  <si>
-    <t>19:40 ⋅ Откроется в 10:00 (чт)</t>
-  </si>
-  <si>
-    <t>La-Dolce-Vita</t>
-  </si>
-  <si>
-    <t>Морская ул., 25</t>
-  </si>
-  <si>
-    <t>Балкон</t>
-  </si>
-  <si>
-    <t>Весенняя ул., 56</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 22:00</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 22:00</t>
-  </si>
-  <si>
-    <t>ТОЧКА.RU</t>
-  </si>
-  <si>
-    <t>ул. Энтузиастов, 11</t>
-  </si>
-  <si>
-    <t>Кафе Замок</t>
-  </si>
-  <si>
-    <t>Весенняя ул., 46а</t>
-  </si>
-  <si>
-    <t>Кумпель</t>
-  </si>
-  <si>
-    <t>8-ая Заводская ул.</t>
-  </si>
-  <si>
-    <t>Открыто ⋅ Закроется в 21:00</t>
-  </si>
-  <si>
-    <t>⋅ Закроется в 21:00</t>
-  </si>
-  <si>
-    <t>Massons</t>
-  </si>
-  <si>
-    <t>ул. Маршала Кошевого, 31</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+  <si>
+    <t>Круглосуточно</t>
+  </si>
+  <si>
+    <t>Йосемити</t>
+  </si>
+  <si>
+    <t>Национальный парк</t>
+  </si>
+  <si>
+    <t>Идеальное место для активного отдыха</t>
+  </si>
+  <si>
+    <t>Йеллоустон</t>
   </si>
   <si>
     <t>Временно закрыто</t>
   </si>
   <si>
-    <t>Империал</t>
-  </si>
-  <si>
-    <t>ул. Маршала Кошевого, 42</t>
-  </si>
-  <si>
-    <t>Виктория</t>
-  </si>
-  <si>
-    <t>б-р Великой Победы, 47А</t>
-  </si>
-  <si>
-    <t>Круглосуточно</t>
-  </si>
-  <si>
-    <t>Resto House</t>
-  </si>
-  <si>
-    <t>ул. Энтузиастов, 9б</t>
-  </si>
-  <si>
-    <t>Чебуречная Ретро</t>
-  </si>
-  <si>
-    <t>пр. Строителей, 12а</t>
-  </si>
-  <si>
-    <t>Кафе Подкова</t>
-  </si>
-  <si>
-    <t>ул. Ленина, 121</t>
+    <t>Национальный парк Гранд Каньон</t>
+  </si>
+  <si>
+    <t>Глубокий каньон с живописными видами</t>
+  </si>
+  <si>
+    <t>Олимпик</t>
+  </si>
+  <si>
+    <t>3002 Mt Angeles Rd</t>
+  </si>
+  <si>
+    <t>Горы, дождевые леса и скалистые берега</t>
+  </si>
+  <si>
+    <t>национальный парк Глейшер</t>
+  </si>
+  <si>
+    <t>Заповедник с более чем 1000 км троп</t>
+  </si>
+  <si>
+    <t>Сейчас открыто</t>
+  </si>
+  <si>
+    <t>Бэдлендс</t>
+  </si>
+  <si>
+    <t>Горные образования и дикая природа</t>
+  </si>
+  <si>
+    <t>Национальный парк Пинаклс</t>
+  </si>
+  <si>
+    <t>Парк с пещерами и скалами</t>
+  </si>
+  <si>
+    <t>Маунт-Рейнир</t>
+  </si>
+  <si>
+    <t>Активный вулкан, ледники и луга</t>
+  </si>
+  <si>
+    <t>Национальный парк Секвойя</t>
+  </si>
+  <si>
+    <t>Огромные деревья, пеший туризм и кемпинг</t>
+  </si>
+  <si>
+    <t>Парк Грэйт Фолс</t>
+  </si>
+  <si>
+    <t>9200 Old Dominion Dr</t>
+  </si>
+  <si>
+    <t>Роки-Маунтин</t>
+  </si>
+  <si>
+    <t>Национальный парк с живописными горами</t>
+  </si>
+  <si>
+    <t>Джошуа-Три</t>
+  </si>
+  <si>
+    <t>Парк в пустыне с необычными скалами</t>
+  </si>
+  <si>
+    <t>Брайс-Каньон</t>
+  </si>
+  <si>
+    <t>Природный амфитеатр и столбы худу</t>
+  </si>
+  <si>
+    <t>Сагуаро</t>
+  </si>
+  <si>
+    <t>Пешие прогулки и пикники среди кактусов</t>
+  </si>
+  <si>
+    <t>Закрыто ⋅ Откроется в 09:00 (пт)</t>
+  </si>
+  <si>
+    <t>Закрыто</t>
+  </si>
+  <si>
+    <t>⋅ Откроется в 09:00 (пт)</t>
+  </si>
+  <si>
+    <t>Парк штата Ниагара-Фолс</t>
+  </si>
+  <si>
+    <t>Парк</t>
+  </si>
+  <si>
+    <t>332 Prospect St</t>
+  </si>
+  <si>
+    <t>Живописный парк с водопадами</t>
+  </si>
+  <si>
+    <t>Редвуд</t>
+  </si>
+  <si>
+    <t>Большой секвойный лес</t>
+  </si>
+  <si>
+    <t>Национальный парк Арчес</t>
+  </si>
+  <si>
+    <t>Походы и кемпинг среди красных скал</t>
+  </si>
+  <si>
+    <t>Национальный парк Долина Смерти</t>
+  </si>
+  <si>
+    <t>Парк площадью больше миллиона гектаров</t>
+  </si>
+  <si>
+    <t>Каньонлендс</t>
+  </si>
+  <si>
+    <t>Живописное место с четырьмя областями</t>
+  </si>
+  <si>
+    <t>Национальный заказник Денали</t>
+  </si>
+  <si>
+    <t>Parks Hwy</t>
+  </si>
+  <si>
+    <t>Парк дикой природы, гора Денали</t>
   </si>
 </sst>
 </file>
@@ -571,399 +535,290 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032A4ACB-EB56-492E-851D-1D485980FE3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D03AA9-6C38-46BA-ADBD-D2B048246F04}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D26AD7-5610-4745-AE78-543DA780FE59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3534D0E-542C-4BD6-A53C-559BEFAC65E8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>